<commit_message>
support more debug error
</commit_message>
<xml_diff>
--- a/Test/Input/SingleTest.xlsx
+++ b/Test/Input/SingleTest.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\MakeConfig.Sharp\Test\Input\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C16FA9-124A-43CB-BC0A-3BACFF01A93E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25820" windowHeight="14620"/>
   </bookViews>
   <sheets>
     <sheet name="SingleTest" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,70 +121,74 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ImportClass3.UintField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定义枚举</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自定义结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导入class类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导入struct类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ImportClass3.FloatField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CustomClass2.StringField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>struct{string name; int Template; enum{X,Y,Z} Location}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1200002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CustomClass2.UlongField</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ulong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string子字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ulong子字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ImportStruct</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ImportClass3.UintField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自定义枚举</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自定义结构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>导入class类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>导入struct类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ImportClass3.FloatField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CustomClass2.StringField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>struct{string name; int Template; enum{X,Y,Z} Location}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1200002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CustomClass2.UlongField</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ulong</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>string子字段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ulong子字段</t>
+    <t>uint</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -502,37 +500,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.08203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,25 +541,25 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="J1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="b">
         <v>1</v>
       </c>
@@ -569,7 +567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -592,24 +590,24 @@
         <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -623,28 +621,28 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -655,7 +653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1200001</v>
       </c>
@@ -669,9 +667,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>

</xml_diff>